<commit_message>
03. 22. -  7:49
</commit_message>
<xml_diff>
--- a/Logiscool/Időnyilvántartás - Március2025.xlsx
+++ b/Logiscool/Időnyilvántartás - Március2025.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,11 +1210,15 @@
       <c r="B22" s="8" t="n">
         <v>45736</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+      <c r="C22" s="9" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D22" s="9" t="n">
+        <v>0.777777777777778</v>
+      </c>
       <c r="E22" s="10" t="n">
         <f aca="false">D22-C22</f>
-        <v>0</v>
+        <v>0.0694444444444445</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1292,7 +1296,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="18" t="n">
         <f aca="false">SUM(E19:E25)</f>
-        <v>0</v>
+        <v>0.0694444444444445</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1547,7 +1551,7 @@
       <c r="D36" s="24"/>
       <c r="E36" s="25" t="n">
         <f aca="false">SUM(E3:E35)</f>
-        <v>0.128472222222222</v>
+        <v>0.197916666666667</v>
       </c>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>

</xml_diff>

<commit_message>
03. 27. - 19:27
</commit_message>
<xml_diff>
--- a/Logiscool/Időnyilvántartás - Március2025.xlsx
+++ b/Logiscool/Időnyilvántartás - Március2025.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24:F25"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1378,11 +1378,15 @@
       <c r="B29" s="8" t="n">
         <v>45743</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+      <c r="C29" s="9" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D29" s="9" t="n">
+        <v>0.774305555555556</v>
+      </c>
       <c r="E29" s="10" t="n">
         <f aca="false">D29-C29</f>
-        <v>0</v>
+        <v>0.0659722222222222</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -1460,7 +1464,7 @@
       <c r="J32" s="15"/>
       <c r="K32" s="18" t="n">
         <f aca="false">SUM(E26:E32)</f>
-        <v>0</v>
+        <v>0.0659722222222222</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1551,7 +1555,7 @@
       <c r="D36" s="24"/>
       <c r="E36" s="25" t="n">
         <f aca="false">SUM(E3:E35)</f>
-        <v>0.197916666666667</v>
+        <v>0.263888888888889</v>
       </c>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>

</xml_diff>